<commit_message>
Uploaded data for participant-2
</commit_message>
<xml_diff>
--- a/data/Collected_traces_output/Execution-Numbers.xlsx
+++ b/data/Collected_traces_output/Execution-Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junayed/Documents/NecessaryDocs/GeorgeMasonUniversity/Research/BugReporting/TraceResults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C35BA9A-3697-F246-AC99-E6FB6FF4A247}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A591A9-8AAD-5841-B676-FFAB9CFB21F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-440" yWindow="800" windowWidth="35840" windowHeight="20720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GNUCASH-2.1.3" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
   <si>
     <t>Execution number</t>
   </si>
@@ -384,10 +384,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -524,6 +524,46 @@
         <v>19</v>
       </c>
     </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -531,10 +571,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5FEB9D-B951-4849-BC6D-655C183F43E8}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -607,6 +647,46 @@
         <v>19</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -614,10 +694,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53BF0B5-0975-0F42-939D-57C0D0B97F6A}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B4:B8"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -688,6 +768,46 @@
       </c>
       <c r="B8" s="4" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded data for evaluation apps - participant 1
</commit_message>
<xml_diff>
--- a/data/Collected_traces_output/Execution-Numbers.xlsx
+++ b/data/Collected_traces_output/Execution-Numbers.xlsx
@@ -5,25 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junayed/Documents/NecessaryDocs/GeorgeMasonUniversity/Research/BugReporting/TraceResults/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junayed/Documents/NecessaryDocs/GeorgeMasonUniversity/Research/BugReporting/BURT-git/burt/data/Collected_traces_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A591A9-8AAD-5841-B676-FFAB9CFB21F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF9A614-61DC-F041-B824-86257D9F355E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GNUCASH-2.1.3" sheetId="1" r:id="rId1"/>
     <sheet name="Antennapod-1.6.2.3" sheetId="2" r:id="rId2"/>
     <sheet name="ATimeTracker-0.20" sheetId="3" r:id="rId3"/>
     <sheet name="GNUCASH-1.0.3" sheetId="4" r:id="rId4"/>
+    <sheet name="token" sheetId="5" r:id="rId5"/>
+    <sheet name="droidweight" sheetId="6" r:id="rId6"/>
+    <sheet name="growtracker" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="27">
   <si>
     <t>Execution number</t>
   </si>
@@ -386,7 +389,7 @@
   </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -820,7 +823,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B6" sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -920,4 +923,205 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7532A6E-3431-B14D-8536-70FDBFE611D3}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A755D77E-D753-F44C-A256-15C1E9F83ED2}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1501879-5621-B948-9648-EC41E16A3BCD}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Uploaded new data for testing
</commit_message>
<xml_diff>
--- a/data/Collected_traces_output/Execution-Numbers.xlsx
+++ b/data/Collected_traces_output/Execution-Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junayed/Documents/NecessaryDocs/GeorgeMasonUniversity/Research/BugReporting/BURT-git/burt/data/Collected_traces_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF9A614-61DC-F041-B824-86257D9F355E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F28EFE-1F60-664C-80D7-4607AA29A60B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6000" yWindow="6980" windowWidth="35840" windowHeight="20720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GNUCASH-2.1.3" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
   <si>
     <t>Execution number</t>
   </si>
@@ -107,6 +107,54 @@
   </si>
   <si>
     <t>P2AppTraces/getevent-5</t>
+  </si>
+  <si>
+    <t>antennapod/getevent-1</t>
+  </si>
+  <si>
+    <t>antennapod/getevent-2</t>
+  </si>
+  <si>
+    <t>antennapod/getevent-3</t>
+  </si>
+  <si>
+    <t>getevent-1</t>
+  </si>
+  <si>
+    <t>getevent-2</t>
+  </si>
+  <si>
+    <t>gnucash-1.0.3/getevent-1</t>
+  </si>
+  <si>
+    <t>gnucash-1.0.3/getevent-2</t>
+  </si>
+  <si>
+    <t>gnucash-1.0.3/getevent-3</t>
+  </si>
+  <si>
+    <t>growtracker-2.3.1/getevent-1</t>
+  </si>
+  <si>
+    <t>growtracker-2.3.1/getevent-2</t>
+  </si>
+  <si>
+    <t>growtracker-2.3.1/getevent-3</t>
+  </si>
+  <si>
+    <t>growtracker-2.3.1/getevent-4</t>
+  </si>
+  <si>
+    <t>growtracker-2.3.1/getevent-5</t>
+  </si>
+  <si>
+    <t>atimetracker/getevent-1</t>
+  </si>
+  <si>
+    <t>token-2.10/getevent-1</t>
+  </si>
+  <si>
+    <t>token-2.10/getevent-2</t>
   </si>
 </sst>
 </file>
@@ -574,10 +622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5FEB9D-B951-4849-BC6D-655C183F43E8}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -690,6 +738,30 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -697,10 +769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53BF0B5-0975-0F42-939D-57C0D0B97F6A}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -813,6 +885,14 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -820,10 +900,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F103F2C-CFD8-4F44-822A-9D522BC3326F}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="A1:B6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -920,6 +1000,30 @@
         <v>26</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -927,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7532A6E-3431-B14D-8536-70FDBFE611D3}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -987,6 +1091,22 @@
         <v>19</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -994,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A755D77E-D753-F44C-A256-15C1E9F83ED2}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1054,6 +1174,22 @@
         <v>19</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1061,16 +1197,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1501879-5621-B948-9648-EC41E16A3BCD}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -1121,6 +1257,46 @@
         <v>19</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>